<commit_message>
Guardando el avance del 21 de febrero
</commit_message>
<xml_diff>
--- a/Curso1 - Curso de Introduccion a Excel/Prueba 1.xlsx
+++ b/Curso1 - Curso de Introduccion a Excel/Prueba 1.xlsx
@@ -5,36 +5,81 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\excelplatzi\Curso1 - Curso de Introduccion a Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DC83F69-4DDC-4D84-8D00-7BD38F93275E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC2E153-1FD9-4B8A-88C4-4AF7E7A22463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{70DF946B-97D1-497C-B545-DE0873EF5DE8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Clientes" sheetId="2" r:id="rId1"/>
+    <sheet name="Ventas" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Platzi</t>
+  </si>
+  <si>
+    <t>Empresa 1</t>
+  </si>
+  <si>
+    <t>Empresa 2</t>
+  </si>
+  <si>
+    <t>Empresa 3</t>
+  </si>
+  <si>
+    <t>Ana Marinez</t>
+  </si>
+  <si>
+    <t>Clientes de mi empresa</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Monto vendido</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,13 +87,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF99FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -60,17 +132,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF99FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -83,7 +175,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -378,13 +470,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A946966-43EC-40EE-BEED-0B8FB903BC60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E16A9C74-D854-4BC9-86F0-71BB94D803AE}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="B1:K13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="205" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5555</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="2">
+        <v>5555</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7777</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2">
+        <v>7777</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2">
+        <v>9999</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8888</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="2">
+        <v>8888</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="I10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="2">
+        <v>5555</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="2">
+        <v>7777</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="I13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="2">
+        <v>8888</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE7AC3C-0008-451D-A93C-7FB007E26753}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="B4:C5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>44562</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A08BB3A-6521-4195-A15F-EF82D32ED8F0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CVentas Mensuales</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>